<commit_message>
more results, add 4 augmentors to file
</commit_message>
<xml_diff>
--- a/data_augmentation/Augmentation Experiment Results.xlsx
+++ b/data_augmentation/Augmentation Experiment Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstra\Documents\GitHub\nuclei\data_augmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3F4C23DB-DBB5-466B-A167-7F4BE30A73C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{09BDF8AC-C9A7-4871-B836-9E0562876A1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8640" windowHeight="210" activeTab="1" xr2:uid="{F804EED9-66D2-473B-B298-A3490873923A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -237,6 +237,39 @@
         iaa.Flipud(1.0),  # vertical flip
         iaa.Multiply((0.5, 1.5), per_channel=0.5),  # lighten or darken
     ])\</t>
+  </si>
+  <si>
+    <t>iaa.SomeOf((0, 2), [
+                iaa.Flipud(1.0),
+                iaa.Multiply((0.5, 1.5), per_channel=0.5),
+                iaa.Affine(shear=(-20, 20)),
+                iaa.Affine(translate_px={"x": (-15, 15), "y": (-15, 15)})
+                ])</t>
+  </si>
+  <si>
+    <t>early stop at 30</t>
+  </si>
+  <si>
+    <t>?early stop at 35ish</t>
+  </si>
+  <si>
+    <t>iaa.SomeOf((0, 2), [
+        iaa.Fliplr(1.0),  # horizontal flip
+        iaa.Flipud(1.0),  # vertical flip
+        iaa.Affine(translate_px={"x": (-15, 15), "y": (-15, 15)}),  # lighten or darken
+    ])</t>
+  </si>
+  <si>
+    <t>early stop at 39</t>
+  </si>
+  <si>
+    <t>iaa.SomeOf((0, 2), [
+                iaa.Flipud(1.0),
+                iaa.Fliplr(1.0),
+                iaa.Multiply((0.5, 1.5), per_channel=0.5),
+                iaa.Affine(shear=(-20, 20)),
+                iaa.Affine(rotate=(-15, 15)),
+                ])</t>
   </si>
 </sst>
 </file>
@@ -627,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CF53CF-3DCD-471C-8B21-E7C555C740F5}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1021,10 +1054,36 @@
       <c r="C37">
         <v>0.58179999999999998</v>
       </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="85.5">
       <c r="A38" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="B38">
+        <v>0.1368</v>
+      </c>
+      <c r="C38">
+        <v>0.51649999999999996</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="85.5">
+      <c r="A39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>8.9099999999999999E-2</v>
+      </c>
+      <c r="C39">
+        <v>0.61729999999999996</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1035,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE8C8E5-84A3-4B5D-8625-D454A46577A7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1360,6 +1419,40 @@
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="B19">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="C19">
+        <v>-0.61680000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="E19">
+        <v>9.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="114">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20">
+        <v>0.186</v>
+      </c>
+      <c r="C20">
+        <v>-0.6996</v>
+      </c>
+      <c r="D20">
+        <v>0.92710000000000004</v>
+      </c>
+      <c r="E20">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="114">
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>